<commit_message>
Updated: to fix the issue with categorization of courses credit types
</commit_message>
<xml_diff>
--- a/ProgrammeCourseDetails.xlsx
+++ b/ProgrammeCourseDetails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicho\Desktop\MyAdvisorContract\myAdvisorDev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39D0580-BEBE-4E42-B14B-D76465A21533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3145526E-9B26-404E-A611-30E5C629BDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-564" yWindow="1068" windowWidth="22824" windowHeight="10512" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11028" yWindow="456" windowWidth="14916" windowHeight="10512" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New Programme Sheet" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2665" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2677" uniqueCount="325">
   <si>
     <t>courseCode</t>
   </si>
@@ -744,9 +744,6 @@
     <t>programmeName</t>
   </si>
   <si>
-    <t>Foun</t>
-  </si>
-  <si>
     <t>Level 1 Elective</t>
   </si>
   <si>
@@ -754,9 +751,6 @@
   </si>
   <si>
     <t>Adv Core</t>
-  </si>
-  <si>
-    <t>Adv CS/IT Elective</t>
   </si>
   <si>
     <t>Adv Elective</t>
@@ -1009,6 +1003,24 @@
   <si>
     <t>Level3Elective</t>
   </si>
+  <si>
+    <t>Total Credits</t>
+  </si>
+  <si>
+    <t>BSc Computer Science (Special) courses amt</t>
+  </si>
+  <si>
+    <t>BSc Computer Scienc With Management (Special)</t>
+  </si>
+  <si>
+    <t>Core Option</t>
+  </si>
+  <si>
+    <t>CIMEM Elective</t>
+  </si>
+  <si>
+    <t>Other Elective</t>
+  </si>
 </sst>
 </file>
 
@@ -1065,7 +1077,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1144,8 +1156,20 @@
         <bgColor rgb="FFF4CCCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1338,11 +1362,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1544,9 +1583,14 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="14" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1563,11 +1607,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1587,10 +1662,16 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="datasheet-style" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="secondRowStripe" dxfId="0"/>
+      <tableStyleElement type="firstRowStripe" dxfId="5"/>
+      <tableStyleElement type="secondRowStripe" dxfId="4"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCCFF"/>
+      <color rgb="FFFF99FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1844,10 +1925,10 @@
   <dimension ref="A1:AE1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="D65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="I36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F70" sqref="F70"/>
+      <selection pane="bottomRight" activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1857,7 +1938,7 @@
     <col min="3" max="3" width="4.77734375" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" customWidth="1"/>
     <col min="5" max="5" width="6.44140625" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
     <col min="7" max="7" width="63.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="11.88671875" customWidth="1"/>
     <col min="10" max="10" width="48.77734375" customWidth="1"/>
@@ -1867,28 +1948,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="13.2">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="86" t="s">
+      <c r="C1" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="86" t="s">
+      <c r="D1" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="86" t="s">
+      <c r="E1" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="86" t="s">
+      <c r="F1" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="G1" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="89" t="s">
+      <c r="H1" s="92" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -1932,14 +2013,14 @@
       <c r="AE1" s="4"/>
     </row>
     <row r="2" spans="1:31" ht="13.2">
-      <c r="A2" s="90"/>
-      <c r="B2" s="90"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
+      <c r="A2" s="93"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
       <c r="I2" s="5" t="s">
         <v>9</v>
       </c>
@@ -1981,14 +2062,14 @@
       <c r="AE2" s="4"/>
     </row>
     <row r="3" spans="1:31" ht="13.2">
-      <c r="A3" s="90"/>
-      <c r="B3" s="90"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
+      <c r="A3" s="93"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
       <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
@@ -2030,14 +2111,14 @@
       <c r="AE3" s="4"/>
     </row>
     <row r="4" spans="1:31" ht="13.2">
-      <c r="A4" s="91"/>
-      <c r="B4" s="91"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
+      <c r="A4" s="94"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
       <c r="I4" s="5" t="s">
         <v>19</v>
       </c>
@@ -2106,16 +2187,16 @@
         <v>27</v>
       </c>
       <c r="K5" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="L5" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M5" s="18" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="N5" s="18" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="O5" s="18" t="s">
         <v>27</v>
@@ -2153,7 +2234,7 @@
         <v>27</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="L6" s="18" t="s">
         <v>27</v>
@@ -2162,7 +2243,7 @@
         <v>27</v>
       </c>
       <c r="N6" s="18" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="O6" s="18" t="s">
         <v>27</v>
@@ -2196,22 +2277,22 @@
       </c>
       <c r="I7" s="23"/>
       <c r="J7" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="L7" s="18" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="M7" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="N7" s="18" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="O7" s="24" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="P7" s="18" t="s">
         <v>27</v>
@@ -2240,25 +2321,25 @@
       </c>
       <c r="I8" s="23"/>
       <c r="J8" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="M8" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="N8" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="O8" s="24" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="P8" s="24" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="T8" s="26">
         <v>3</v>
@@ -2290,25 +2371,25 @@
       </c>
       <c r="I9" s="23"/>
       <c r="J9" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="K9" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="L9" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="M9" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="N9" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="O9" s="24" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="P9" s="24" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="T9" s="26">
         <v>4</v>
@@ -2340,22 +2421,22 @@
       </c>
       <c r="I10" s="23"/>
       <c r="J10" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="L10" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="M10" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="N10" s="18" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="O10" s="24" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="P10" s="18" t="s">
         <v>27</v>
@@ -2392,22 +2473,22 @@
       </c>
       <c r="I11" s="23"/>
       <c r="J11" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="K11" s="18" t="s">
         <v>27</v>
       </c>
       <c r="L11" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="M11" s="28" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="N11" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="O11" s="29" t="s">
         <v>27</v>
-      </c>
-      <c r="O11" s="29" t="s">
-        <v>44</v>
       </c>
       <c r="P11" s="18" t="s">
         <v>27</v>
@@ -2441,19 +2522,19 @@
         <v>28</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="L12" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M12" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="N12" s="18" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="O12" s="24" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="P12" s="18" t="s">
         <v>27</v>
@@ -2492,19 +2573,19 @@
         <v>28</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="L13" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M13" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="N13" s="18" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="O13" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="P13" s="18" t="s">
         <v>27</v>
@@ -2544,22 +2625,22 @@
         <v>28</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="L14" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="M14" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="N14" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="O14" s="24" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="P14" s="18" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:31" ht="13.2">
@@ -2590,19 +2671,19 @@
         <v>28</v>
       </c>
       <c r="K15" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="L15" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M15" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="N15" s="18" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="O15" s="30" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="P15" s="18" t="s">
         <v>27</v>
@@ -2636,22 +2717,22 @@
         <v>28</v>
       </c>
       <c r="K16" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="L16" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="M16" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="N16" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="O16" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="P16" s="24" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="13.2">
@@ -2682,19 +2763,19 @@
         <v>28</v>
       </c>
       <c r="K17" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="L17" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="M17" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="N17" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="O17" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="P17" s="18" t="s">
         <v>27</v>
@@ -2728,19 +2809,19 @@
         <v>28</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="L18" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M18" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="N18" s="18" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="O18" s="24" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="P18" s="18" t="s">
         <v>27</v>
@@ -2771,22 +2852,22 @@
       </c>
       <c r="I19" s="23"/>
       <c r="J19" s="19" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="K19" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="L19" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M19" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="N19" s="18" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="O19" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="P19" s="18" t="s">
         <v>27</v>
@@ -2817,22 +2898,22 @@
       </c>
       <c r="I20" s="23"/>
       <c r="J20" s="19" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="K20" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="L20" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M20" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="N20" s="18" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="O20" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="P20" s="18" t="s">
         <v>27</v>
@@ -2863,22 +2944,22 @@
       </c>
       <c r="I21" s="23"/>
       <c r="J21" s="19" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="K21" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="L21" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="M21" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="N21" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="O21" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="P21" s="18" t="s">
         <v>27</v>
@@ -2909,25 +2990,25 @@
       </c>
       <c r="I22" s="23"/>
       <c r="J22" s="34" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="K22" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="L22" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="M22" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="N22" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="O22" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="P22" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="26.4">
@@ -2955,22 +3036,22 @@
       </c>
       <c r="I23" s="23"/>
       <c r="J23" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="K23" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="L23" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M23" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="N23" s="18" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="O23" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="P23" s="18" t="s">
         <v>27</v>
@@ -3001,22 +3082,22 @@
       </c>
       <c r="I24" s="23"/>
       <c r="J24" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="K24" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="L24" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="M24" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="N24" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="O24" s="18" t="s">
-        <v>27</v>
+        <v>245</v>
       </c>
       <c r="P24" s="18" t="s">
         <v>27</v>
@@ -3047,22 +3128,22 @@
       </c>
       <c r="I25" s="23"/>
       <c r="J25" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="K25" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="L25" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M25" s="18" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="N25" s="18" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="O25" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="P25" s="18" t="s">
         <v>27</v>
@@ -3093,22 +3174,22 @@
       </c>
       <c r="I26" s="23"/>
       <c r="J26" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="K26" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="L26" s="31" t="s">
-        <v>52</v>
+        <v>247</v>
       </c>
       <c r="M26" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="N26" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="O26" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="P26" s="18" t="s">
         <v>27</v>
@@ -3139,25 +3220,25 @@
       </c>
       <c r="I27" s="23"/>
       <c r="J27" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="K27" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="L27" s="31" t="s">
-        <v>52</v>
+        <v>247</v>
       </c>
       <c r="M27" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="N27" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="O27" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="P27" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="13.2">
@@ -3185,22 +3266,22 @@
       </c>
       <c r="I28" s="23"/>
       <c r="J28" s="19" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="K28" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="L28" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M28" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="N28" s="18" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="O28" s="18" t="s">
-        <v>27</v>
+        <v>245</v>
       </c>
       <c r="P28" s="18" t="s">
         <v>27</v>
@@ -3234,19 +3315,19 @@
         <v>27</v>
       </c>
       <c r="K29" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="L29" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M29" s="18" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="N29" s="18" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="O29" s="18" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="P29" s="18" t="s">
         <v>27</v>
@@ -3280,19 +3361,19 @@
         <v>27</v>
       </c>
       <c r="K30" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="L30" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M30" s="18" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="N30" s="18" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="O30" s="18" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="P30" s="18" t="s">
         <v>27</v>
@@ -3321,25 +3402,25 @@
       </c>
       <c r="I31" s="23"/>
       <c r="J31" s="39" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="K31" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="L31" s="40" t="s">
-        <v>100</v>
+        <v>39</v>
+      </c>
+      <c r="L31" s="88" t="s">
+        <v>39</v>
       </c>
       <c r="M31" s="18" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="N31" s="18" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="O31" s="18" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="P31" s="18" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="26.4">
@@ -3367,25 +3448,25 @@
       </c>
       <c r="I32" s="23"/>
       <c r="J32" s="39" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="K32" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="L32" s="40" t="s">
-        <v>100</v>
+        <v>39</v>
+      </c>
+      <c r="L32" s="88" t="s">
+        <v>39</v>
       </c>
       <c r="M32" s="18" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="N32" s="18" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="O32" s="18" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="P32" s="18" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="28.8">
@@ -3413,25 +3494,25 @@
       </c>
       <c r="I33" s="23"/>
       <c r="J33" s="39" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="K33" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="L33" s="40" t="s">
-        <v>100</v>
+        <v>39</v>
+      </c>
+      <c r="L33" s="88" t="s">
+        <v>39</v>
       </c>
       <c r="M33" s="18" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="N33" s="18" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="O33" s="18" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="P33" s="18" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="26.4">
@@ -3459,25 +3540,25 @@
       </c>
       <c r="I34" s="23"/>
       <c r="J34" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="K34" s="18" t="s">
         <v>27</v>
       </c>
       <c r="L34" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="M34" s="28" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="N34" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="O34" s="18" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="P34" s="24" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="26.4">
@@ -3505,25 +3586,25 @@
       </c>
       <c r="I35" s="23"/>
       <c r="J35" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="K35" s="18" t="s">
         <v>27</v>
       </c>
       <c r="L35" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="M35" s="28" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="N35" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="O35" s="18" t="s">
         <v>27</v>
       </c>
       <c r="P35" s="24" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="28.8">
@@ -3554,22 +3635,22 @@
         <v>27</v>
       </c>
       <c r="K36" s="18" t="s">
-        <v>27</v>
+        <v>246</v>
       </c>
       <c r="L36" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="M36" s="18" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="N36" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="O36" s="18" t="s">
         <v>27</v>
       </c>
       <c r="P36" s="24" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="26.4">
@@ -3600,22 +3681,22 @@
         <v>27</v>
       </c>
       <c r="K37" s="18" t="s">
-        <v>27</v>
+        <v>246</v>
       </c>
       <c r="L37" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="M37" s="18" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="N37" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="O37" s="18" t="s">
         <v>27</v>
       </c>
       <c r="P37" s="24" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:21" ht="26.4">
@@ -3646,22 +3727,22 @@
         <v>28</v>
       </c>
       <c r="K38" s="31" t="s">
-        <v>52</v>
+        <v>246</v>
       </c>
       <c r="L38" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="M38" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="N38" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="O38" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="P38" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
     </row>
     <row r="39" spans="1:21" ht="13.2">
@@ -3692,22 +3773,22 @@
         <v>27</v>
       </c>
       <c r="K39" s="18" t="s">
-        <v>27</v>
+        <v>246</v>
       </c>
       <c r="L39" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="M39" s="14" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="N39" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="O39" s="18" t="s">
         <v>27</v>
       </c>
       <c r="P39" s="24" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:21" ht="26.4">
@@ -3738,22 +3819,22 @@
         <v>28</v>
       </c>
       <c r="K40" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="L40" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="M40" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="N40" s="19" t="s">
-        <v>28</v>
+        <v>158</v>
       </c>
       <c r="O40" s="18" t="s">
-        <v>27</v>
+        <v>245</v>
       </c>
       <c r="P40" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="26.4">
@@ -3781,25 +3862,25 @@
       </c>
       <c r="I41" s="23"/>
       <c r="J41" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="K41" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="L41" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="M41" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="N41" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="O41" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="P41" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
     </row>
     <row r="42" spans="1:21" ht="26.4">
@@ -3827,22 +3908,22 @@
       </c>
       <c r="I42" s="23"/>
       <c r="J42" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="K42" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="L42" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="M42" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="N42" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="O42" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="P42" s="18" t="s">
         <v>27</v>
@@ -3876,16 +3957,16 @@
         <v>27</v>
       </c>
       <c r="K43" s="18" t="s">
-        <v>27</v>
+        <v>246</v>
       </c>
       <c r="L43" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="M43" s="18" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="N43" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="O43" s="18" t="s">
         <v>27</v>
@@ -3922,19 +4003,19 @@
         <v>27</v>
       </c>
       <c r="K44" s="18" t="s">
-        <v>27</v>
+        <v>246</v>
       </c>
       <c r="L44" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="M44" s="18" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="N44" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="O44" s="18" t="s">
-        <v>27</v>
+        <v>245</v>
       </c>
       <c r="P44" s="18" t="s">
         <v>27</v>
@@ -3965,22 +4046,22 @@
       </c>
       <c r="I45" s="23"/>
       <c r="J45" s="19" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="K45" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="L45" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="M45" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="N45" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="O45" s="30" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="P45" s="18" t="s">
         <v>27</v>
@@ -4011,25 +4092,25 @@
       </c>
       <c r="I46" s="23"/>
       <c r="J46" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="K46" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="L46" s="31" t="s">
-        <v>52</v>
+        <v>247</v>
       </c>
       <c r="M46" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="N46" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="O46" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="P46" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
     </row>
     <row r="47" spans="1:21" ht="13.2">
@@ -4057,25 +4138,25 @@
       </c>
       <c r="I47" s="23"/>
       <c r="J47" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="K47" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="L47" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="M47" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="N47" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="O47" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="P47" s="30" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="T47" s="26" t="s">
         <v>145</v>
@@ -4109,25 +4190,25 @@
       </c>
       <c r="I48" s="23"/>
       <c r="J48" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="K48" s="31" t="s">
-        <v>52</v>
+        <v>246</v>
       </c>
       <c r="L48" s="31" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="M48" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="N48" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="O48" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="P48" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
     </row>
     <row r="49" spans="1:16" ht="13.2">
@@ -4155,25 +4236,25 @@
       </c>
       <c r="I49" s="23"/>
       <c r="J49" s="42" t="s">
-        <v>28</v>
+        <v>158</v>
       </c>
       <c r="K49" s="18" t="s">
-        <v>27</v>
+        <v>245</v>
       </c>
       <c r="L49" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="M49" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="N49" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="O49" s="18" t="s">
-        <v>27</v>
+        <v>245</v>
       </c>
       <c r="P49" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="14.4">
@@ -4201,25 +4282,25 @@
       </c>
       <c r="I50" s="23"/>
       <c r="J50" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="K50" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="L50" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="M50" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="N50" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="O50" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="P50" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="14.4">
@@ -4247,25 +4328,25 @@
       </c>
       <c r="I51" s="23"/>
       <c r="J51" s="31" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="K51" s="43" t="s">
         <v>158</v>
       </c>
       <c r="L51" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="M51" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="N51" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="O51" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="P51" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
     </row>
     <row r="52" spans="1:16" ht="13.2">
@@ -4293,25 +4374,25 @@
       </c>
       <c r="I52" s="17"/>
       <c r="J52" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="K52" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="L52" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="K52" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="L52" s="31" t="s">
-        <v>52</v>
-      </c>
       <c r="M52" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="N52" s="31" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="O52" s="30" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="P52" s="30" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:16" ht="26.4">
@@ -4337,20 +4418,22 @@
       </c>
       <c r="I53" s="23"/>
       <c r="J53" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="K53" s="17"/>
+        <v>52</v>
+      </c>
+      <c r="K53" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="L53" s="19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="M53" s="28" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="N53" s="18" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="O53" s="29" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="P53" s="18" t="s">
         <v>27</v>
@@ -4384,22 +4467,22 @@
         <v>28</v>
       </c>
       <c r="K54" s="14" t="s">
-        <v>52</v>
+        <v>247</v>
       </c>
       <c r="L54" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="M54" s="31" t="s">
-        <v>52</v>
+        <v>247</v>
       </c>
       <c r="N54" s="31" t="s">
-        <v>52</v>
+        <v>247</v>
       </c>
       <c r="O54" s="30" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="P54" s="30" t="s">
-        <v>52</v>
+        <v>247</v>
       </c>
     </row>
     <row r="55" spans="1:16" ht="13.2">
@@ -4430,16 +4513,16 @@
         <v>27</v>
       </c>
       <c r="K55" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="L55" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M55" s="18" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="N55" s="18" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="O55" s="18" t="s">
         <v>27</v>
@@ -4476,16 +4559,16 @@
         <v>27</v>
       </c>
       <c r="K56" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="L56" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M56" s="18" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="N56" s="18" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="O56" s="18" t="s">
         <v>27</v>
@@ -4522,16 +4605,16 @@
         <v>27</v>
       </c>
       <c r="K57" s="19" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="L57" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M57" s="18" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="N57" s="18" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="O57" s="18" t="s">
         <v>27</v>
@@ -4725,10 +4808,17 @@
       <c r="C70" s="46"/>
       <c r="D70" s="47"/>
       <c r="E70" s="46"/>
-      <c r="F70" s="48"/>
-      <c r="G70" s="85"/>
-      <c r="H70" s="48"/>
+      <c r="F70" s="85"/>
+      <c r="G70" s="86" t="s">
+        <v>320</v>
+      </c>
+      <c r="H70" s="85" t="s">
+        <v>319</v>
+      </c>
       <c r="J70" s="48"/>
+      <c r="K70" t="s">
+        <v>321</v>
+      </c>
       <c r="L70" s="45"/>
       <c r="M70" s="50"/>
       <c r="N70" s="45"/>
@@ -4740,10 +4830,23 @@
       <c r="C71" s="46"/>
       <c r="D71" s="47"/>
       <c r="E71" s="46"/>
-      <c r="F71" s="48"/>
-      <c r="G71" s="49"/>
-      <c r="H71" s="48"/>
+      <c r="F71" s="85" t="str">
+        <f>'Programme Credits'!$F$1</f>
+        <v>Level 1 Core</v>
+      </c>
+      <c r="G71" s="87">
+        <f>COUNTIF($J$5:$J$57, $F71)</f>
+        <v>8</v>
+      </c>
+      <c r="H71" s="85">
+        <f>PRODUCT($G71, 3)</f>
+        <v>24</v>
+      </c>
       <c r="J71" s="48"/>
+      <c r="K71">
+        <f>COUNTIF($K$5:$K$57, $F71)</f>
+        <v>8</v>
+      </c>
       <c r="L71" s="45"/>
       <c r="M71" s="50"/>
       <c r="N71" s="45"/>
@@ -4755,9 +4858,22 @@
       <c r="C72" s="46"/>
       <c r="D72" s="47"/>
       <c r="E72" s="46"/>
-      <c r="F72" s="48"/>
-      <c r="G72" s="49"/>
-      <c r="H72" s="48"/>
+      <c r="F72" s="85" t="str">
+        <f>'Programme Credits'!$G$1</f>
+        <v>Level 2 Core</v>
+      </c>
+      <c r="G72" s="87">
+        <f t="shared" ref="G72:G79" si="0">COUNTIF($J$5:$J$57, $F72)</f>
+        <v>10</v>
+      </c>
+      <c r="H72" s="85">
+        <f>PRODUCT($G72, 3)</f>
+        <v>30</v>
+      </c>
+      <c r="K72">
+        <f t="shared" ref="K72:K80" si="1">COUNTIF($K$5:$K$57, $F72)</f>
+        <v>0</v>
+      </c>
       <c r="L72" s="45"/>
       <c r="M72" s="50"/>
       <c r="N72" s="45"/>
@@ -4769,10 +4885,23 @@
       <c r="C73" s="46"/>
       <c r="D73" s="47"/>
       <c r="E73" s="46"/>
-      <c r="F73" s="48"/>
-      <c r="G73" s="49"/>
-      <c r="H73" s="48"/>
+      <c r="F73" s="85" t="str">
+        <f>'Programme Credits'!$H$1</f>
+        <v>Level 3 Core</v>
+      </c>
+      <c r="G73" s="87">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H73" s="85">
+        <f t="shared" ref="H73:H79" si="2">PRODUCT($G73, 3)</f>
+        <v>15</v>
+      </c>
       <c r="J73" s="48"/>
+      <c r="K73">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L73" s="45"/>
       <c r="M73" s="50"/>
       <c r="N73" s="45"/>
@@ -4784,10 +4913,23 @@
       <c r="C74" s="46"/>
       <c r="D74" s="47"/>
       <c r="E74" s="46"/>
-      <c r="F74" s="48"/>
-      <c r="G74" s="49"/>
-      <c r="H74" s="48"/>
+      <c r="F74" s="85" t="str">
+        <f>'Programme Credits'!$C$1</f>
+        <v>Foundation</v>
+      </c>
+      <c r="G74" s="87">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H74" s="85">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
       <c r="J74" s="48"/>
+      <c r="K74">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="L74" s="45"/>
       <c r="M74" s="50"/>
       <c r="N74" s="45"/>
@@ -4799,10 +4941,23 @@
       <c r="C75" s="46"/>
       <c r="D75" s="47"/>
       <c r="E75" s="46"/>
-      <c r="F75" s="48"/>
-      <c r="G75" s="49"/>
-      <c r="H75" s="48"/>
+      <c r="F75" s="85" t="str">
+        <f>'Programme Credits'!$D$1</f>
+        <v>Level 1 Elective</v>
+      </c>
+      <c r="G75" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H75" s="85">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="J75" s="48"/>
+      <c r="K75">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L75" s="45"/>
       <c r="M75" s="50"/>
       <c r="N75" s="45"/>
@@ -4814,10 +4969,23 @@
       <c r="C76" s="46"/>
       <c r="D76" s="47"/>
       <c r="E76" s="46"/>
-      <c r="F76" s="48"/>
-      <c r="G76" s="49"/>
-      <c r="H76" s="48"/>
+      <c r="F76" s="85" t="str">
+        <f>'Programme Credits'!$E$1</f>
+        <v>Level 1 CS/IT Core</v>
+      </c>
+      <c r="G76" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H76" s="85">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="J76" s="48"/>
+      <c r="K76">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L76" s="45"/>
       <c r="M76" s="50"/>
       <c r="N76" s="45"/>
@@ -4829,10 +4997,22 @@
       <c r="C77" s="46"/>
       <c r="D77" s="47"/>
       <c r="E77" s="46"/>
-      <c r="F77" s="48"/>
-      <c r="G77" s="49"/>
-      <c r="H77" s="48"/>
+      <c r="F77" s="85" t="s">
+        <v>49</v>
+      </c>
+      <c r="G77" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H77" s="85">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="J77" s="48"/>
+      <c r="K77">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
       <c r="L77" s="45"/>
       <c r="M77" s="50"/>
       <c r="N77" s="45"/>
@@ -4844,10 +5024,23 @@
       <c r="C78" s="46"/>
       <c r="D78" s="47"/>
       <c r="E78" s="46"/>
-      <c r="F78" s="48"/>
-      <c r="G78" s="49"/>
-      <c r="H78" s="48"/>
+      <c r="F78" s="85" t="str">
+        <f>'Programme Credits'!$J$1</f>
+        <v>Advanced Elective CS/IT</v>
+      </c>
+      <c r="G78" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H78" s="85">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="J78" s="48"/>
+      <c r="K78">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
       <c r="L78" s="45"/>
       <c r="M78" s="50"/>
       <c r="N78" s="45"/>
@@ -4859,10 +5052,23 @@
       <c r="C79" s="46"/>
       <c r="D79" s="47"/>
       <c r="E79" s="46"/>
-      <c r="F79" s="48"/>
-      <c r="G79" s="49"/>
-      <c r="H79" s="48"/>
+      <c r="F79" s="85" t="str">
+        <f>'Programme Credits'!$K$1</f>
+        <v>Adv Elective</v>
+      </c>
+      <c r="G79" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H79" s="85">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="J79" s="48"/>
+      <c r="K79">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L79" s="45"/>
       <c r="M79" s="50"/>
       <c r="N79" s="45"/>
@@ -4874,10 +5080,22 @@
       <c r="C80" s="46"/>
       <c r="D80" s="47"/>
       <c r="E80" s="46"/>
-      <c r="F80" s="48"/>
-      <c r="G80" s="49"/>
-      <c r="H80" s="48"/>
+      <c r="F80" s="85" t="s">
+        <v>27</v>
+      </c>
+      <c r="G80" s="87">
+        <f>COUNTIF($J$5:$J$57, $F80)</f>
+        <v>12</v>
+      </c>
+      <c r="H80" s="85">
+        <f>IF($F$80="N/A", 0, PRODUCT($G80, 3))</f>
+        <v>0</v>
+      </c>
       <c r="J80" s="48"/>
+      <c r="K80">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="L80" s="45"/>
       <c r="M80" s="50"/>
       <c r="N80" s="45"/>
@@ -4889,9 +5107,17 @@
       <c r="C81" s="46"/>
       <c r="D81" s="47"/>
       <c r="E81" s="46"/>
-      <c r="F81" s="48"/>
-      <c r="G81" s="49"/>
-      <c r="H81" s="48"/>
+      <c r="F81" s="85" t="s">
+        <v>158</v>
+      </c>
+      <c r="G81" s="87">
+        <f>COUNTIF($J$5:$J$57, $F81)</f>
+        <v>15</v>
+      </c>
+      <c r="H81" s="85">
+        <f>PRODUCT($G81, 3)</f>
+        <v>45</v>
+      </c>
       <c r="J81" s="48"/>
       <c r="L81" s="45"/>
       <c r="M81" s="50"/>
@@ -4904,9 +5130,9 @@
       <c r="C82" s="46"/>
       <c r="D82" s="47"/>
       <c r="E82" s="46"/>
-      <c r="F82" s="48"/>
-      <c r="G82" s="49"/>
-      <c r="H82" s="48"/>
+      <c r="F82" s="85"/>
+      <c r="G82" s="87"/>
+      <c r="H82" s="85"/>
       <c r="J82" s="48"/>
       <c r="L82" s="45"/>
       <c r="M82" s="50"/>
@@ -4919,9 +5145,15 @@
       <c r="C83" s="46"/>
       <c r="D83" s="47"/>
       <c r="E83" s="46"/>
-      <c r="F83" s="48"/>
-      <c r="G83" s="49"/>
-      <c r="H83" s="48"/>
+      <c r="F83" s="85"/>
+      <c r="G83" s="87">
+        <f>SUM($G71:$G80)</f>
+        <v>38</v>
+      </c>
+      <c r="H83" s="85">
+        <f>SUM(H71:H81)</f>
+        <v>123</v>
+      </c>
       <c r="J83" s="48"/>
       <c r="L83" s="45"/>
       <c r="M83" s="50"/>
@@ -18725,8 +18957,28 @@
     <mergeCell ref="D1:D4"/>
     <mergeCell ref="E1:E4"/>
   </mergeCells>
+  <conditionalFormatting sqref="G71">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="notEqual">
+      <formula>8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G72">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G73">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G74">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J5:P30 J31:K33 M31:P33 J34:P52 J53 L53:P53 J54:P57" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J5:P57" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Advanced Core,Advanced Elective CS/IT,Advanced Elective CS/IT/Econ/MATH/Mgmt,Advanced Elective CS/IT/MATH,Advanced General Elective,Foundation,Level 1 Core,Level 2 Core,Level 3 Core,N/A"</formula1>
     </dataValidation>
   </dataValidations>
@@ -18743,7 +18995,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -18765,13 +19017,13 @@
         <v>233</v>
       </c>
       <c r="C1" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="46" t="s">
         <v>234</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="E1" s="46" t="s">
         <v>235</v>
-      </c>
-      <c r="E1" s="46" t="s">
-        <v>236</v>
       </c>
       <c r="F1" s="46" t="s">
         <v>52</v>
@@ -18783,16 +19035,16 @@
         <v>44</v>
       </c>
       <c r="I1" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="J1" s="46" t="s">
+        <v>245</v>
+      </c>
+      <c r="K1" s="46" t="s">
         <v>237</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="L1" s="46" t="s">
         <v>238</v>
-      </c>
-      <c r="K1" s="46" t="s">
-        <v>239</v>
-      </c>
-      <c r="L1" s="46" t="s">
-        <v>240</v>
       </c>
       <c r="M1" s="65"/>
       <c r="N1" s="46"/>
@@ -19219,7 +19471,7 @@
   <dimension ref="A1:AE1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="G15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="G46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="J30" sqref="J30"/>
@@ -19241,28 +19493,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="13.2">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="86" t="s">
+      <c r="C1" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="86" t="s">
+      <c r="D1" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="86" t="s">
+      <c r="E1" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="86" t="s">
+      <c r="F1" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="G1" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="89" t="s">
+      <c r="H1" s="92" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -19306,14 +19558,14 @@
       <c r="AE1" s="4"/>
     </row>
     <row r="2" spans="1:31" ht="13.2">
-      <c r="A2" s="90"/>
-      <c r="B2" s="90"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
+      <c r="A2" s="93"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
       <c r="I2" s="5" t="s">
         <v>9</v>
       </c>
@@ -19355,14 +19607,14 @@
       <c r="AE2" s="4"/>
     </row>
     <row r="3" spans="1:31" ht="13.2">
-      <c r="A3" s="90"/>
-      <c r="B3" s="90"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
+      <c r="A3" s="93"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
       <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
@@ -19404,14 +19656,14 @@
       <c r="AE3" s="4"/>
     </row>
     <row r="4" spans="1:31" ht="13.2">
-      <c r="A4" s="91"/>
-      <c r="B4" s="91"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
+      <c r="A4" s="94"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
       <c r="I4" s="5" t="s">
         <v>19</v>
       </c>
@@ -39712,11 +39964,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D2" sqref="D2"/>
+      <selection pane="topRight" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -39728,7 +39980,7 @@
     <col min="5" max="5" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:5">
       <c r="B1" s="69" t="s">
         <v>232</v>
       </c>
@@ -39742,38 +39994,38 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:5">
       <c r="B2" s="69" t="s">
         <v>233</v>
       </c>
       <c r="C2" s="72" t="s">
+        <v>239</v>
+      </c>
+      <c r="D2" s="71" t="s">
+        <v>240</v>
+      </c>
+      <c r="E2" s="73" t="s">
         <v>241</v>
       </c>
-      <c r="D2" s="71" t="s">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="74" t="s">
         <v>242</v>
       </c>
-      <c r="E2" s="73" t="s">
+      <c r="B3" s="74" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="74" t="s">
+      <c r="C3" s="75" t="s">
         <v>244</v>
       </c>
-      <c r="B3" s="74" t="s">
-        <v>245</v>
-      </c>
-      <c r="C3" s="75" t="s">
-        <v>246</v>
-      </c>
       <c r="D3" s="75" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E3" s="76" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="77">
         <v>1</v>
       </c>
@@ -39790,7 +40042,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:5">
       <c r="A5" s="71">
         <v>2</v>
       </c>
@@ -39807,7 +40059,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:5">
       <c r="A6" s="71">
         <v>3</v>
       </c>
@@ -39820,7 +40072,7 @@
       <c r="D6" s="71"/>
       <c r="E6" s="64"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:5">
       <c r="A7" s="71">
         <v>4</v>
       </c>
@@ -39833,7 +40085,7 @@
       </c>
       <c r="E7" s="64"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:5">
       <c r="A8" s="71">
         <v>5</v>
       </c>
@@ -39848,7 +40100,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:5">
       <c r="A9" s="71">
         <v>6</v>
       </c>
@@ -39863,12 +40115,12 @@
       </c>
       <c r="E9" s="64"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:5">
       <c r="A10" s="71">
         <v>7</v>
       </c>
       <c r="B10" s="71" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C10" s="71"/>
       <c r="D10" s="71">
@@ -39878,12 +40130,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:5">
       <c r="A11" s="71">
         <v>8</v>
       </c>
       <c r="B11" s="71" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C11" s="64"/>
       <c r="D11" s="71">
@@ -39891,96 +40143,151 @@
       </c>
       <c r="E11" s="71"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:5">
       <c r="A12" s="71">
         <v>9</v>
       </c>
       <c r="B12" s="71" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C12" s="64"/>
       <c r="D12" s="71"/>
       <c r="E12" s="71"/>
     </row>
-    <row r="13" spans="1:10">
-      <c r="B13" s="81" t="s">
-        <v>250</v>
-      </c>
-      <c r="C13" s="71">
+    <row r="13" spans="1:5">
+      <c r="A13" s="99">
+        <v>10</v>
+      </c>
+      <c r="B13" s="99" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="64"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="99">
+        <v>11</v>
+      </c>
+      <c r="B14" s="99" t="s">
+        <v>322</v>
+      </c>
+      <c r="C14" s="64"/>
+      <c r="D14" s="71"/>
+      <c r="E14" s="71"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="99">
+        <v>12</v>
+      </c>
+      <c r="B15" s="99" t="s">
+        <v>323</v>
+      </c>
+      <c r="C15" s="64"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="71"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="99">
+        <v>13</v>
+      </c>
+      <c r="B16" s="99" t="s">
+        <v>324</v>
+      </c>
+      <c r="C16" s="64"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="71"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="99">
+        <v>14</v>
+      </c>
+      <c r="B17" s="99" t="s">
+        <v>237</v>
+      </c>
+      <c r="C17" s="64"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="B18" s="81" t="s">
+        <v>248</v>
+      </c>
+      <c r="C18" s="71">
         <f>SUM(C4:C9)</f>
         <v>93</v>
       </c>
-      <c r="D13" s="71">
+      <c r="D18" s="71">
         <f>SUM(D4:D12)</f>
         <v>93</v>
       </c>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="71"/>
-      <c r="J13" s="71"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="26" t="s">
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="71"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="26" t="s">
         <v>251</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B22" s="26" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="26" t="s">
+    <row r="23" spans="1:10">
+      <c r="A23" s="26" t="s">
         <v>253</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B23" s="26" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="26" t="s">
+    <row r="24" spans="1:10">
+      <c r="A24" s="26" t="s">
         <v>255</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B24" s="26" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="26" t="s">
+    <row r="25" spans="1:10">
+      <c r="A25" s="26" t="s">
         <v>257</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B25" s="26" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="26" t="s">
+    <row r="26" spans="1:10">
+      <c r="A26" s="26" t="s">
         <v>259</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B26" s="26" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="26" t="s">
-        <v>261</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>262</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B4:B12" xr:uid="{00000000-0002-0000-0500-000000000000}">
-      <formula1>"Advanced Core,Advanced Elective CS/IT,Advanced Elective CS/IT/Econ/MATH/Mgmt,Advanced Elective CS/IT/MATH,Advanced General Elective,Foundation,Level 1 Core,Level 2 Core,Level 3 Core"</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B4:B17" xr:uid="{00000000-0002-0000-0500-000000000000}">
+      <formula1>"Advanced Core,Advanced Elective CS/IT,Advanced Elective CS/IT/Econ/MATH/Mgmt,Advanced Elective CS/IT/MATH,Advanced General Elective,Foundation,Level 1 Core,Level 2 Core,Level 3 Core,L1 Elective, Core Option, Other Elective,Adv Elective,CIMEM Elective"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -40004,56 +40311,56 @@
   <sheetData>
     <row r="2" spans="1:6">
       <c r="A2" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>263</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>264</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="26" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="26" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="26" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="26" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="B8" s="26" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="96" t="s">
+        <v>270</v>
+      </c>
+      <c r="B9" s="97"/>
+      <c r="D9" s="96" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="93" t="s">
-        <v>272</v>
-      </c>
-      <c r="B9" s="94"/>
-      <c r="D9" s="93" t="s">
-        <v>273</v>
-      </c>
-      <c r="E9" s="95"/>
-      <c r="F9" s="94"/>
+      <c r="E9" s="98"/>
+      <c r="F9" s="97"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="64" t="s">
@@ -40077,7 +40384,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="64" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C11" s="82"/>
       <c r="D11" s="83" t="s">
@@ -40087,7 +40394,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="64" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -40095,7 +40402,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="64" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D12" s="64" t="s">
         <v>227</v>
@@ -40104,7 +40411,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="64" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -40112,7 +40419,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="64" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D13" s="64" t="s">
         <v>227</v>
@@ -40121,7 +40428,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="64" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -40129,7 +40436,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="64" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D14" s="64" t="s">
         <v>87</v>
@@ -40138,7 +40445,7 @@
         <v>3</v>
       </c>
       <c r="F14" s="64" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -40146,7 +40453,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="64" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D15" s="64" t="s">
         <v>153</v>
@@ -40155,7 +40462,7 @@
         <v>2</v>
       </c>
       <c r="F15" s="64" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -40166,15 +40473,15 @@
         <v>4</v>
       </c>
       <c r="F16" s="64" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="50" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D17" s="64" t="s">
         <v>153</v>
@@ -40183,15 +40490,15 @@
         <v>2</v>
       </c>
       <c r="F17" s="64" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="50" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D18" s="64" t="s">
         <v>153</v>
@@ -40200,15 +40507,15 @@
         <v>4</v>
       </c>
       <c r="F18" s="64" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="50" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -40221,7 +40528,7 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="26" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -40263,25 +40570,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="13.2">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="86" t="s">
+      <c r="C1" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="86" t="s">
+      <c r="D1" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="86" t="s">
+      <c r="E1" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="86" t="s">
+      <c r="F1" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="G1" s="92" t="s">
         <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -40325,13 +40632,13 @@
       <c r="AD1" s="4"/>
     </row>
     <row r="2" spans="1:30" ht="13.2">
-      <c r="A2" s="90"/>
-      <c r="B2" s="90"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="90"/>
+      <c r="A2" s="93"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="93"/>
       <c r="H2" s="5" t="s">
         <v>9</v>
       </c>
@@ -40373,13 +40680,13 @@
       <c r="AD2" s="4"/>
     </row>
     <row r="3" spans="1:30" ht="13.2">
-      <c r="A3" s="90"/>
-      <c r="B3" s="90"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="90"/>
+      <c r="A3" s="93"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="93"/>
       <c r="H3" s="5" t="s">
         <v>17</v>
       </c>
@@ -40421,13 +40728,13 @@
       <c r="AD3" s="4"/>
     </row>
     <row r="4" spans="1:30" ht="28.2" customHeight="1">
-      <c r="A4" s="91"/>
-      <c r="B4" s="91"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="91"/>
+      <c r="A4" s="94"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="94"/>
       <c r="H4" s="5" t="s">
         <v>19</v>
       </c>
@@ -40485,7 +40792,7 @@
         <v>25</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G5" s="16" t="s">
         <v>26</v>
@@ -40533,7 +40840,7 @@
         <v>25</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G6" s="16"/>
       <c r="H6" s="17"/>
@@ -40579,7 +40886,7 @@
         <v>25</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G7" s="16"/>
       <c r="H7" s="23"/>
@@ -40633,7 +40940,7 @@
         <v>25</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G8" s="16"/>
       <c r="H8" s="23"/>
@@ -40691,7 +40998,7 @@
         <v>25</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G9" s="16"/>
       <c r="H9" s="23"/>
@@ -40749,7 +41056,7 @@
         <v>25</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G10" s="16"/>
       <c r="H10" s="23"/>
@@ -40803,7 +41110,7 @@
         <v>25</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G11" s="16"/>
       <c r="H11" s="23"/>
@@ -40855,21 +41162,21 @@
         <v>25</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G12" s="16"/>
       <c r="H12" s="23"/>
       <c r="I12" s="19" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J12" s="18"/>
       <c r="K12" s="52"/>
       <c r="L12" s="55" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M12" s="52"/>
       <c r="N12" s="55" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="O12" s="52"/>
       <c r="P12" s="26"/>
@@ -40905,21 +41212,21 @@
         <v>25</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G13" s="16"/>
       <c r="H13" s="26"/>
       <c r="I13" s="19" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J13" s="18"/>
       <c r="K13" s="52"/>
       <c r="L13" s="55" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M13" s="52"/>
       <c r="N13" s="58" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O13" s="52"/>
       <c r="P13" s="26"/>
@@ -40955,27 +41262,27 @@
         <v>25</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="23"/>
       <c r="I14" s="19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J14" s="51" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K14" s="55" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="L14" s="55" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="M14" s="58" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="N14" s="55" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O14" s="52"/>
       <c r="P14" s="26"/>
@@ -41011,23 +41318,23 @@
         <v>25</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="23"/>
       <c r="I15" s="19" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J15" s="51" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="K15" s="53"/>
       <c r="L15" s="56" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M15" s="53"/>
       <c r="N15" s="56" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="O15" s="53"/>
       <c r="P15" s="26"/>
@@ -41063,28 +41370,28 @@
         <v>25</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="23"/>
       <c r="I16" s="19" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="J16" s="17"/>
       <c r="K16" s="19" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="L16" s="51" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="M16" s="19" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="N16" s="59" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="O16" s="19" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="P16" s="26"/>
       <c r="Q16" s="26"/>
@@ -41119,18 +41426,18 @@
         <v>25</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G17" s="16"/>
       <c r="H17" s="23"/>
       <c r="I17" s="19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J17" s="60" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="K17" s="55" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="L17" s="58" t="s">
         <v>175</v>
@@ -41175,12 +41482,12 @@
         <v>25</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G18" s="16"/>
       <c r="H18" s="23"/>
       <c r="I18" s="19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J18" s="17"/>
       <c r="K18" s="52"/>
@@ -41225,15 +41532,15 @@
         <v>25</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G19" s="16"/>
       <c r="H19" s="23"/>
       <c r="I19" s="19" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="J19" s="60" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="K19" s="52"/>
       <c r="L19" s="60" t="s">
@@ -41277,15 +41584,15 @@
         <v>25</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G20" s="16"/>
       <c r="H20" s="23"/>
       <c r="I20" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="J20" s="60" t="s">
         <v>293</v>
-      </c>
-      <c r="J20" s="60" t="s">
-        <v>295</v>
       </c>
       <c r="K20" s="52"/>
       <c r="L20" s="58" t="s">
@@ -41329,18 +41636,18 @@
         <v>25</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G21" s="16"/>
       <c r="H21" s="23"/>
       <c r="I21" s="19" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J21" s="31" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="K21" s="55" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="L21" s="58" t="s">
         <v>181</v>
@@ -41385,18 +41692,18 @@
         <v>25</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G22" s="16"/>
       <c r="H22" s="23"/>
       <c r="I22" s="31" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J22" s="31" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K22" s="58" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="L22" s="58" t="s">
         <v>182</v>
@@ -41443,7 +41750,7 @@
         <v>25</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G23" s="16"/>
       <c r="H23" s="23"/>
@@ -41495,18 +41802,18 @@
         <v>25</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G24" s="16"/>
       <c r="H24" s="23"/>
       <c r="I24" s="31" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="J24" s="60" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="K24" s="58" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="L24" s="59" t="s">
         <v>184</v>
@@ -41551,15 +41858,15 @@
         <v>25</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G25" s="16"/>
       <c r="H25" s="23"/>
       <c r="I25" s="31" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="J25" s="60" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="K25" s="52"/>
       <c r="L25" s="53"/>
@@ -41601,15 +41908,15 @@
         <v>25</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G26" s="16"/>
       <c r="H26" s="23"/>
       <c r="I26" s="31" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J26" s="60" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="K26" s="31" t="s">
         <v>187</v>
@@ -41657,7 +41964,7 @@
         <v>25</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G27" s="16"/>
       <c r="H27" s="23"/>
@@ -41715,15 +42022,15 @@
         <v>25</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G28" s="16"/>
       <c r="H28" s="23"/>
       <c r="I28" s="19" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J28" s="60" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="K28" s="52"/>
       <c r="L28" s="59" t="s">
@@ -41765,7 +42072,7 @@
         <v>25</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G29" s="16"/>
       <c r="H29" s="17"/>
@@ -41811,7 +42118,7 @@
         <v>25</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G30" s="16"/>
       <c r="H30" s="17"/>
@@ -41857,7 +42164,7 @@
         <v>25</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G31" s="16"/>
       <c r="H31" s="23"/>
@@ -41907,7 +42214,7 @@
         <v>25</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G32" s="16"/>
       <c r="H32" s="23"/>
@@ -41945,7 +42252,7 @@
         <v>103</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C33" s="38" t="s">
         <v>23</v>
@@ -41957,7 +42264,7 @@
         <v>25</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G33" s="16"/>
       <c r="H33" s="23"/>
@@ -42007,7 +42314,7 @@
         <v>25</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G34" s="16"/>
       <c r="H34" s="23"/>
@@ -42061,7 +42368,7 @@
         <v>25</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G35" s="16"/>
       <c r="H35" s="23"/>
@@ -42115,7 +42422,7 @@
         <v>25</v>
       </c>
       <c r="F36" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G36" s="16"/>
       <c r="H36" s="17"/>
@@ -42165,7 +42472,7 @@
         <v>25</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G37" s="14" t="s">
         <v>57</v>
@@ -42217,15 +42524,15 @@
         <v>25</v>
       </c>
       <c r="F38" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G38" s="16"/>
       <c r="H38" s="23"/>
       <c r="I38" s="19" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J38" s="31" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="K38" s="55" t="s">
         <v>191</v>
@@ -42275,7 +42582,7 @@
         <v>25</v>
       </c>
       <c r="F39" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G39" s="14" t="s">
         <v>45</v>
@@ -42327,15 +42634,15 @@
         <v>25</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G40" s="16"/>
       <c r="H40" s="23"/>
       <c r="I40" s="19" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="J40" s="60" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="K40" s="55" t="s">
         <v>194</v>
@@ -42385,15 +42692,15 @@
         <v>25</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G41" s="16"/>
       <c r="H41" s="23"/>
       <c r="I41" s="31" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J41" s="60" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="K41" s="55" t="s">
         <v>197</v>
@@ -42443,7 +42750,7 @@
         <v>25</v>
       </c>
       <c r="F42" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G42" s="16"/>
       <c r="H42" s="23"/>
@@ -42499,7 +42806,7 @@
         <v>25</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G43" s="16"/>
       <c r="H43" s="17"/>
@@ -42518,10 +42825,10 @@
       <c r="Q43" s="26"/>
       <c r="R43" s="26"/>
       <c r="S43" s="46" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="T43" s="46" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="U43" s="26"/>
       <c r="V43" s="26"/>
@@ -42551,7 +42858,7 @@
         <v>25</v>
       </c>
       <c r="F44" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G44" s="16"/>
       <c r="H44" s="17"/>
@@ -42573,7 +42880,7 @@
         <v>1</v>
       </c>
       <c r="T44" s="46" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="U44" s="26"/>
       <c r="V44" s="26"/>
@@ -42603,7 +42910,7 @@
         <v>25</v>
       </c>
       <c r="F45" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G45" s="16"/>
       <c r="H45" s="23"/>
@@ -42633,7 +42940,7 @@
         <v>2</v>
       </c>
       <c r="T45" s="46" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="U45" s="26"/>
       <c r="V45" s="26"/>
@@ -42663,17 +42970,17 @@
         <v>25</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G46" s="16" t="s">
         <v>141</v>
       </c>
       <c r="H46" s="23"/>
       <c r="I46" s="31" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="J46" s="60" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="K46" s="31" t="s">
         <v>206</v>
@@ -42697,7 +43004,7 @@
         <v>3</v>
       </c>
       <c r="T46" s="46" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="U46" s="26"/>
       <c r="V46" s="26"/>
@@ -42727,7 +43034,7 @@
         <v>25</v>
       </c>
       <c r="F47" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G47" s="16"/>
       <c r="H47" s="23"/>
@@ -42738,19 +43045,19 @@
         <v>198</v>
       </c>
       <c r="K47" s="31" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="L47" s="60" t="s">
+        <v>311</v>
+      </c>
+      <c r="M47" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="N47" s="60" t="s">
         <v>313</v>
       </c>
-      <c r="M47" s="31" t="s">
+      <c r="O47" s="31" t="s">
         <v>314</v>
-      </c>
-      <c r="N47" s="60" t="s">
-        <v>315</v>
-      </c>
-      <c r="O47" s="31" t="s">
-        <v>316</v>
       </c>
       <c r="P47" s="26"/>
       <c r="Q47" s="26"/>
@@ -42759,7 +43066,7 @@
         <v>4</v>
       </c>
       <c r="T47" s="46" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="U47" s="26"/>
       <c r="V47" s="26"/>
@@ -42789,17 +43096,17 @@
         <v>25</v>
       </c>
       <c r="F48" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G48" s="16" t="s">
         <v>141</v>
       </c>
       <c r="H48" s="23"/>
       <c r="I48" s="31" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="J48" s="60" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="K48" s="31" t="s">
         <v>209</v>
@@ -42823,7 +43130,7 @@
         <v>5</v>
       </c>
       <c r="T48" s="46" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="U48" s="26"/>
       <c r="V48" s="26"/>
@@ -42853,7 +43160,7 @@
         <v>25</v>
       </c>
       <c r="F49" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G49" s="16"/>
       <c r="H49" s="23"/>
@@ -42881,7 +43188,7 @@
         <v>6</v>
       </c>
       <c r="T49" s="46" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="U49" s="26"/>
       <c r="V49" s="26"/>
@@ -42911,7 +43218,7 @@
         <v>25</v>
       </c>
       <c r="F50" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G50" s="16"/>
       <c r="H50" s="23"/>
@@ -42973,7 +43280,7 @@
         <v>157</v>
       </c>
       <c r="F51" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G51" s="16"/>
       <c r="H51" s="23"/>
@@ -43031,7 +43338,7 @@
         <v>25</v>
       </c>
       <c r="F52" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G52" s="16"/>
       <c r="H52" s="17"/>
@@ -43087,7 +43394,7 @@
         <v>25</v>
       </c>
       <c r="F53" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G53" s="16"/>
       <c r="H53" s="23"/>
@@ -43139,7 +43446,7 @@
         <v>25</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G54" s="16"/>
       <c r="H54" s="23"/>
@@ -43197,7 +43504,7 @@
         <v>25</v>
       </c>
       <c r="F55" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G55" s="16"/>
       <c r="H55" s="17"/>
@@ -43243,7 +43550,7 @@
         <v>25</v>
       </c>
       <c r="F56" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G56" s="16"/>
       <c r="H56" s="17"/>
@@ -43289,7 +43596,7 @@
         <v>25</v>
       </c>
       <c r="F57" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G57" s="16"/>
       <c r="H57" s="17"/>

</xml_diff>